<commit_message>
Stage before returning to two squation solution
</commit_message>
<xml_diff>
--- a/results/tables/final_tables.xlsx
+++ b/results/tables/final_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C02C9A-80C6-4E3D-B116-4C38C7A12FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AE4A1A-9F09-49F5-8FF8-495B1079FE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={5FB4546E-B91B-4CDE-868E-4F97C041A2D6}</author>
-    <author>tc={2AF38892-021B-43B5-AF10-FE5CA22CE887}</author>
+    <author>tc={D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}</author>
     <author>tc={134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}</author>
   </authors>
   <commentList>
@@ -92,13 +92,13 @@
     I have to correct this. I just realized a variable had the wrong sign</t>
       </text>
     </comment>
-    <comment ref="A10" authorId="1" shapeId="0" xr:uid="{2AF38892-021B-43B5-AF10-FE5CA22CE887}">
+    <comment ref="A10" authorId="1" shapeId="0" xr:uid="{D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}">
       <text>
-        <t>[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    I need to verify I can reproduce these results.
-It should be fine, but just to be safe</t>
+    In production. Panicking a little bit
+</t>
       </text>
     </comment>
     <comment ref="D17" authorId="2" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="99">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -433,6 +433,9 @@
   <si>
     <t>Not winsorized</t>
   </si>
+  <si>
+    <t>Skill acquisition costs estimates :(</t>
+  </si>
 </sst>
 </file>
 
@@ -441,9 +444,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000_);\(0.0000\)"/>
+    <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,12 +498,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -677,29 +674,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -717,9 +693,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -728,6 +704,27 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1065,12 +1062,12 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2023-05-04T14:24:46.91" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{5FB4546E-B91B-4CDE-868E-4F97C041A2D6}">
+  <threadedComment ref="A1" dT="2023-05-04T14:24:46.91" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{5FB4546E-B91B-4CDE-868E-4F97C041A2D6}" done="1">
     <text>I have to correct this. I just realized a variable had the wrong sign</text>
   </threadedComment>
-  <threadedComment ref="A10" dT="2023-05-04T10:49:17.95" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{2AF38892-021B-43B5-AF10-FE5CA22CE887}">
-    <text>I need to verify I can reproduce these results.
-It should be fine, but just to be safe</text>
+  <threadedComment ref="A10" dT="2023-05-05T16:03:41.57" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}">
+    <text xml:space="preserve">In production. Panicking a little bit
+</text>
   </threadedComment>
   <threadedComment ref="D17" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
     <text>Should I winsorize it?</text>
@@ -1096,14 +1093,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
@@ -1138,7 +1135,7 @@
       <c r="E3" s="9">
         <v>0.44195289999999998</v>
       </c>
-      <c r="J3" s="40"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1156,7 +1153,7 @@
       <c r="E4" s="9">
         <v>0.53484730000000003</v>
       </c>
-      <c r="J4" s="40"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -1174,7 +1171,7 @@
       <c r="E5" s="9">
         <v>0.62221070000000001</v>
       </c>
-      <c r="J5" s="40"/>
+      <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
@@ -1192,7 +1189,7 @@
       <c r="E6" s="11">
         <v>0.23334750000000001</v>
       </c>
-      <c r="J6" s="40"/>
+      <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -1204,12 +1201,12 @@
       <c r="E7" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
@@ -1523,13 +1520,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1701,16 +1698,16 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="25" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1743,55 +1740,55 @@
     <col min="14" max="14" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="14.54296875" customWidth="1"/>
     <col min="20" max="20" width="17.08984375" customWidth="1"/>
-    <col min="21" max="28" width="11.90625" style="34" customWidth="1"/>
+    <col min="21" max="28" width="11.90625" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="35"/>
     </row>
     <row r="2" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="46"/>
-      <c r="B2" s="45" t="s">
+      <c r="A2" s="39"/>
+      <c r="B2" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="38" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="37"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="3" t="s">
         <v>70</v>
       </c>
@@ -1811,7 +1808,7 @@
         <v>75</v>
       </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="37"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="3" t="s">
         <v>66</v>
       </c>
@@ -1824,379 +1821,379 @@
       <c r="R2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="T2" s="33"/>
-      <c r="U2" s="35" t="s">
+      <c r="T2" s="26"/>
+      <c r="U2" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="V2" s="35" t="s">
+      <c r="V2" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="W2" s="35" t="s">
+      <c r="W2" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="X2" s="35" t="s">
+      <c r="X2" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="Y2" s="35" t="s">
+      <c r="Y2" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="Z2" s="35" t="s">
+      <c r="Z2" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="AA2" s="35" t="s">
+      <c r="AA2" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="AB2" s="35" t="s">
+      <c r="AB2" s="28" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="31">
         <v>1</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="F3" s="36" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="F3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="31">
         <v>1</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="N3" s="36" t="s">
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="N3" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="38">
+      <c r="O3" s="31">
         <v>1</v>
       </c>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="T3" s="36" t="s">
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="T3" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="U3" s="39">
+      <c r="U3" s="32">
         <v>1</v>
       </c>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="39"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="31">
         <v>0.51829999999999998</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="31">
         <v>1</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="F4" s="36" t="s">
+      <c r="D4" s="31"/>
+      <c r="F4" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="31">
         <v>0.25540000000000002</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="31">
         <v>1</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="N4" s="36" t="s">
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="N4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="O4" s="38">
+      <c r="O4" s="31">
         <v>4.3900000000000002E-2</v>
       </c>
-      <c r="P4" s="38">
+      <c r="P4" s="31">
         <v>1</v>
       </c>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="T4" s="36" t="s">
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="T4" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="U4" s="39">
+      <c r="U4" s="32">
         <v>0.63819999999999999</v>
       </c>
-      <c r="V4" s="39">
+      <c r="V4" s="32">
         <v>1</v>
       </c>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="39"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="32"/>
+      <c r="AB4" s="32"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="31">
         <v>0.50839999999999996</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="31">
         <v>0.76880000000000004</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="31">
         <v>1</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="31">
         <v>0.28789999999999999</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="31">
         <v>0.63729999999999998</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="31">
         <v>1</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="N5" s="36" t="s">
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="N5" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="O5" s="38">
+      <c r="O5" s="31">
         <v>0.2888</v>
       </c>
-      <c r="P5" s="38">
+      <c r="P5" s="31">
         <v>0.2281</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="31">
         <v>1</v>
       </c>
-      <c r="R5" s="38"/>
-      <c r="T5" s="36" t="s">
+      <c r="R5" s="31"/>
+      <c r="T5" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="U5" s="39">
+      <c r="U5" s="32">
         <v>0.21809999999999999</v>
       </c>
-      <c r="V5" s="39">
+      <c r="V5" s="32">
         <v>0.23069999999999999</v>
       </c>
-      <c r="W5" s="39">
+      <c r="W5" s="32">
         <v>1</v>
       </c>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="39"/>
-      <c r="AB5" s="39"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="32"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="31">
         <v>0.26</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="31">
         <v>0.25380000000000003</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="31">
         <v>0.25659999999999999</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="31">
         <v>1</v>
       </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="N6" s="36" t="s">
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="N6" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="38">
+      <c r="O6" s="31">
         <v>0.13589999999999999</v>
       </c>
-      <c r="P6" s="38">
+      <c r="P6" s="31">
         <v>0.25690000000000002</v>
       </c>
-      <c r="Q6" s="38">
+      <c r="Q6" s="31">
         <v>0.3261</v>
       </c>
-      <c r="R6" s="38">
+      <c r="R6" s="31">
         <v>1</v>
       </c>
-      <c r="T6" s="36" t="s">
+      <c r="T6" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="U6" s="39">
+      <c r="U6" s="32">
         <v>0.30109999999999998</v>
       </c>
-      <c r="V6" s="39">
+      <c r="V6" s="32">
         <v>0.29310000000000003</v>
       </c>
-      <c r="W6" s="39">
+      <c r="W6" s="32">
         <v>0.74509999999999998</v>
       </c>
-      <c r="X6" s="39">
+      <c r="X6" s="32">
         <v>1</v>
       </c>
-      <c r="Y6" s="39"/>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="39"/>
-      <c r="AB6" s="39"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="32"/>
+      <c r="AB6" s="32"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="31">
         <v>0.35020000000000001</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="31">
         <v>0.30549999999999999</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="31">
         <v>0.32550000000000001</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="31">
         <v>0.58360000000000001</v>
       </c>
-      <c r="K7" s="38">
+      <c r="K7" s="31">
         <v>1</v>
       </c>
-      <c r="L7" s="38"/>
-      <c r="T7" s="36" t="s">
+      <c r="L7" s="31"/>
+      <c r="T7" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="U7" s="39">
+      <c r="U7" s="32">
         <v>0.36630000000000001</v>
       </c>
-      <c r="V7" s="39">
+      <c r="V7" s="32">
         <v>0.33350000000000002</v>
       </c>
-      <c r="W7" s="39">
+      <c r="W7" s="32">
         <v>0.50819999999999999</v>
       </c>
-      <c r="X7" s="39">
+      <c r="X7" s="32">
         <v>0.66100000000000003</v>
       </c>
-      <c r="Y7" s="39">
+      <c r="Y7" s="32">
         <v>1</v>
       </c>
-      <c r="Z7" s="39"/>
-      <c r="AA7" s="39"/>
-      <c r="AB7" s="39"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="32"/>
+      <c r="AB7" s="32"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="31">
         <v>0.29680000000000001</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="31">
         <v>0.4209</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="31">
         <v>0.39650000000000002</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="31">
         <v>0.43440000000000001</v>
       </c>
-      <c r="K8" s="38">
+      <c r="K8" s="31">
         <v>0.46660000000000001</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="31">
         <v>1</v>
       </c>
-      <c r="T8" s="36" t="s">
+      <c r="T8" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="U8" s="39">
+      <c r="U8" s="32">
         <v>0.36059999999999998</v>
       </c>
-      <c r="V8" s="39">
+      <c r="V8" s="32">
         <v>0.33729999999999999</v>
       </c>
-      <c r="W8" s="39">
+      <c r="W8" s="32">
         <v>0.17580000000000001</v>
       </c>
-      <c r="X8" s="39">
+      <c r="X8" s="32">
         <v>0.2117</v>
       </c>
-      <c r="Y8" s="39">
+      <c r="Y8" s="32">
         <v>0.23380000000000001</v>
       </c>
-      <c r="Z8" s="39">
+      <c r="Z8" s="32">
         <v>1</v>
       </c>
-      <c r="AA8" s="39"/>
-      <c r="AB8" s="39"/>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="32"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="T9" s="36" t="s">
+      <c r="T9" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="U9" s="39">
+      <c r="U9" s="32">
         <v>0.31609999999999999</v>
       </c>
-      <c r="V9" s="39">
+      <c r="V9" s="32">
         <v>0.3785</v>
       </c>
-      <c r="W9" s="39">
+      <c r="W9" s="32">
         <v>0.26490000000000002</v>
       </c>
-      <c r="X9" s="39">
+      <c r="X9" s="32">
         <v>0.29549999999999998</v>
       </c>
-      <c r="Y9" s="39">
+      <c r="Y9" s="32">
         <v>0.26300000000000001</v>
       </c>
-      <c r="Z9" s="39">
+      <c r="Z9" s="32">
         <v>0.34379999999999999</v>
       </c>
-      <c r="AA9" s="39">
+      <c r="AA9" s="32">
         <v>1</v>
       </c>
-      <c r="AB9" s="39"/>
+      <c r="AB9" s="32"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="T10" s="36" t="s">
+      <c r="T10" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="U10" s="39">
+      <c r="U10" s="32">
         <v>0.48359999999999997</v>
       </c>
-      <c r="V10" s="39">
+      <c r="V10" s="32">
         <v>0.51070000000000004</v>
       </c>
-      <c r="W10" s="39">
+      <c r="W10" s="32">
         <v>0.25890000000000002</v>
       </c>
-      <c r="X10" s="39">
+      <c r="X10" s="32">
         <v>0.34379999999999999</v>
       </c>
-      <c r="Y10" s="39">
+      <c r="Y10" s="32">
         <v>0.40450000000000003</v>
       </c>
-      <c r="Z10" s="39">
+      <c r="Z10" s="32">
         <v>0.37290000000000001</v>
       </c>
-      <c r="AA10" s="39">
+      <c r="AA10" s="32">
         <v>0.59109999999999996</v>
       </c>
-      <c r="AB10" s="39">
+      <c r="AB10" s="32">
         <v>1</v>
       </c>
     </row>
@@ -2226,14 +2223,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
@@ -2305,16 +2302,16 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="36">
         <v>-5.7299999999999999E-3</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="36">
         <v>-3.8400000000000001E-3</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="36">
         <v>-5.4099999999999999E-3</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="36">
         <v>-4.5700000000000003E-3</v>
       </c>
     </row>
@@ -2341,16 +2338,16 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="36">
         <v>-8.8000000000000005E-3</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="36">
         <v>-4.6100000000000004E-3</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="36">
         <v>-5.1900000000000002E-3</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="36">
         <v>-4.9500000000000004E-3</v>
       </c>
     </row>
@@ -2377,16 +2374,16 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B13" s="43">
+      <c r="B13" s="36">
         <v>-3.8600000000000001E-3</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="36">
         <v>-2.2799999999999999E-3</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="36">
         <v>-2.8500000000000001E-3</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="36">
         <v>-2.49E-3</v>
       </c>
     </row>
@@ -2444,13 +2441,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2470,8 +2467,8 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2481,21 +2478,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="44"/>
+      <c r="A1" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2527,63 +2524,87 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="G4" s="20" t="e">
+      <c r="B4" s="9">
+        <v>0.24072823758123699</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.36823580676442402</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.767879233440253</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.21333003904938899</v>
+      </c>
+      <c r="G4" s="20">
         <f>+C4/$B4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" s="20" t="e">
+        <v>1.529674335110595</v>
+      </c>
+      <c r="H4" s="20">
         <f t="shared" ref="H4:I6" si="0">+D4/$B4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" s="20" t="e">
+        <v>3.1898178674660955</v>
+      </c>
+      <c r="I4" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.88618618734911769</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="G5" s="20" t="e">
+      <c r="B5" s="9">
+        <v>0.24072823758123699</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.19519018525746901</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.64705534179666802</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.53952349185391701</v>
+      </c>
+      <c r="G5" s="20">
         <f t="shared" ref="G5:G6" si="1">+C5/$B5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" s="20" t="e">
+        <v>0.8108321118398063</v>
+      </c>
+      <c r="H5" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I5" s="20" t="e">
+        <v>2.6879079425749151</v>
+      </c>
+      <c r="I5" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.2412139816869119</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="G6" s="20" t="e">
+      <c r="B6" s="23">
+        <v>0.24072823758123699</v>
+      </c>
+      <c r="C6" s="23">
+        <v>0.72144995745774898</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0.43889801398964001</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0.11339157652500501</v>
+      </c>
+      <c r="G6" s="20">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="20" t="e">
+        <v>2.9969477810607321</v>
+      </c>
+      <c r="H6" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" s="20" t="e">
+        <v>1.8232095179175978</v>
+      </c>
+      <c r="I6" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.47103562782799624</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2604,20 +2625,20 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
@@ -2654,15 +2675,15 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="G13" s="20" t="e">
-        <f>+C13/$B13</f>
+        <f t="shared" ref="G13:I15" si="2">+C13/$B13</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H13" s="20" t="e">
-        <f>+D13/$B13</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I13" s="20" t="e">
-        <f>+E13/$B13</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2675,15 +2696,15 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="G14" s="20" t="e">
-        <f>+C14/$B14</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H14" s="20" t="e">
-        <f>+D14/$B14</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I14" s="20" t="e">
-        <f>+E14/$B14</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2696,15 +2717,15 @@
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
       <c r="G15" s="20" t="e">
-        <f>+C15/$B15</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H15" s="20" t="e">
-        <f>+D15/$B15</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I15" s="20" t="e">
-        <f>+E15/$B15</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added three-equation weighted solution
</commit_message>
<xml_diff>
--- a/results/tables/final_tables.xlsx
+++ b/results/tables/final_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AE4A1A-9F09-49F5-8FF8-495B1079FE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6406EF1-7276-4811-BF8C-9807EE8FC063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
@@ -81,6 +81,7 @@
   <authors>
     <author>tc={5FB4546E-B91B-4CDE-868E-4F97C041A2D6}</author>
     <author>tc={D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}</author>
+    <author>tc={CF4562D9-D2D5-4667-BC22-6D1B99AEC1C0}</author>
     <author>tc={134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}</author>
   </authors>
   <commentList>
@@ -101,7 +102,16 @@
 </t>
       </text>
     </comment>
-    <comment ref="D17" authorId="2" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+    <comment ref="A19" authorId="2" shapeId="0" xr:uid="{CF4562D9-D2D5-4667-BC22-6D1B99AEC1C0}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In production. Panicking a little bit
+</t>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="3" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -114,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="99">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -1069,7 +1079,11 @@
     <text xml:space="preserve">In production. Panicking a little bit
 </text>
   </threadedComment>
-  <threadedComment ref="D17" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+  <threadedComment ref="A19" dT="2023-05-05T16:03:41.57" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{CF4562D9-D2D5-4667-BC22-6D1B99AEC1C0}">
+    <text xml:space="preserve">In production. Panicking a little bit
+</text>
+  </threadedComment>
+  <threadedComment ref="D26" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
     <text>Should I winsorize it?</text>
   </threadedComment>
 </ThreadedComments>
@@ -2465,10 +2479,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2477,7 +2491,7 @@
     <col min="2" max="5" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="46" t="s">
         <v>98</v>
       </c>
@@ -2485,7 +2499,7 @@
       <c r="C1" s="46"/>
       <c r="D1" s="46"/>
       <c r="E1" s="46"/>
-      <c r="F1" s="37"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G2" s="45" t="s">
@@ -2632,6 +2646,7 @@
       <c r="C10" s="46"/>
       <c r="D10" s="46"/>
       <c r="E10" s="46"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G11" s="45" t="s">
@@ -2670,87 +2685,244 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="G13" s="20" t="e">
+      <c r="B13" s="9">
+        <v>0.27885169368546697</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.30320567448449298</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.233826029968141</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.91303831241435396</v>
+      </c>
+      <c r="G13" s="20">
         <f t="shared" ref="G13:I15" si="2">+C13/$B13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" s="20" t="e">
+        <v>1.087336678781289</v>
+      </c>
+      <c r="H13" s="20">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" s="20" t="e">
+        <v>0.83853186214420838</v>
+      </c>
+      <c r="I13" s="20">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>3.2742792426580092</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="G14" s="20" t="e">
+      <c r="B14" s="9">
+        <v>0.27885169368546697</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.188967867153742</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.79801410460793898</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.30461932615272902</v>
+      </c>
+      <c r="G14" s="20">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="20" t="e">
+        <v>0.67766440524793747</v>
+      </c>
+      <c r="H14" s="20">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" s="20" t="e">
+        <v>2.8617868303431049</v>
+      </c>
+      <c r="I14" s="20">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1.0924062254265052</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="G15" s="20" t="e">
+      <c r="B15" s="23">
+        <v>0.27885169368546697</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0.82120048408405799</v>
+      </c>
+      <c r="D15" s="23">
+        <v>0.190953511290265</v>
+      </c>
+      <c r="E15" s="23">
+        <v>0.25665144370672199</v>
+      </c>
+      <c r="G15" s="20">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="20" t="e">
+        <v>2.9449363323944437</v>
+      </c>
+      <c r="H15" s="20">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="20" t="e">
+        <v>0.68478519447564323</v>
+      </c>
+      <c r="I15" s="20">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.92038689209545943</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="37"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
+  <conditionalFormatting sqref="G13:G15">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:H15">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:I15">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G6">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H6">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Added sigma parameter estimates
</commit_message>
<xml_diff>
--- a/results/tables/final_tables.xlsx
+++ b/results/tables/final_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6406EF1-7276-4811-BF8C-9807EE8FC063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAEC78B-737D-4D39-9B32-5ABACB0483A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
@@ -81,7 +81,6 @@
   <authors>
     <author>tc={5FB4546E-B91B-4CDE-868E-4F97C041A2D6}</author>
     <author>tc={D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}</author>
-    <author>tc={CF4562D9-D2D5-4667-BC22-6D1B99AEC1C0}</author>
     <author>tc={134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}</author>
   </authors>
   <commentList>
@@ -102,16 +101,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="A19" authorId="2" shapeId="0" xr:uid="{CF4562D9-D2D5-4667-BC22-6D1B99AEC1C0}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    In production. Panicking a little bit
-</t>
-      </text>
-    </comment>
-    <comment ref="D26" authorId="3" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+    <comment ref="D26" authorId="2" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -124,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="102">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -446,6 +436,15 @@
   <si>
     <t>Skill acquisition costs estimates :(</t>
   </si>
+  <si>
+    <t>Different manual</t>
+  </si>
+  <si>
+    <t>Skill acquisition costs estimates :)</t>
+  </si>
+  <si>
+    <t>Skill acquisition costs estimates :|</t>
+  </si>
 </sst>
 </file>
 
@@ -456,7 +455,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,12 +503,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -523,7 +516,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,12 +538,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -703,12 +690,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -721,7 +707,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1079,10 +1065,6 @@
     <text xml:space="preserve">In production. Panicking a little bit
 </text>
   </threadedComment>
-  <threadedComment ref="A19" dT="2023-05-05T16:03:41.57" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{CF4562D9-D2D5-4667-BC22-6D1B99AEC1C0}">
-    <text xml:space="preserve">In production. Panicking a little bit
-</text>
-  </threadedComment>
   <threadedComment ref="D26" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
     <text>Should I winsorize it?</text>
   </threadedComment>
@@ -1107,13 +1089,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
       <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1215,12 +1197,12 @@
       <c r="E7" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
@@ -1534,12 +1516,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1758,47 +1740,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
       <c r="AC1" s="35"/>
     </row>
     <row r="2" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="39"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="37" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="1"/>
@@ -2237,13 +2219,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2455,13 +2437,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2479,10 +2461,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2492,21 +2474,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2639,21 +2621,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G11" s="45" t="s">
+      <c r="G11" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
@@ -2768,7 +2750,7 @@
         <v>0.92038689209545943</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2785,18 +2767,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="46" t="s">
+    <row r="19" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="37"/>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G20" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
@@ -2812,35 +2800,104 @@
       <c r="E21" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="9">
+        <v>0.28041979658886301</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.41399915754056499</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.69763918662608104</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.20209181959310901</v>
+      </c>
+      <c r="G22" s="20">
+        <f t="shared" ref="G22:G24" si="3">+C22/$B22</f>
+        <v>1.476354959873069</v>
+      </c>
+      <c r="H22" s="20">
+        <f t="shared" ref="H22:H24" si="4">+D22/$B22</f>
+        <v>2.4878385731408383</v>
+      </c>
+      <c r="I22" s="20">
+        <f t="shared" ref="I22:I24" si="5">+E22/$B22</f>
+        <v>0.72067600808300125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="9">
+        <v>0.28041979658886301</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.52861914399065901</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.55762567138944696</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.21526761088893601</v>
+      </c>
+      <c r="G23" s="20">
+        <f t="shared" si="3"/>
+        <v>1.88509923486498</v>
+      </c>
+      <c r="H23" s="20">
+        <f t="shared" si="4"/>
+        <v>1.9885388912360167</v>
+      </c>
+      <c r="I23" s="20">
+        <f t="shared" si="5"/>
+        <v>0.76766196077287019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="23">
+        <v>0.28041979658886301</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0.69713513547848305</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.37707053835847798</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.16923062066442399</v>
+      </c>
+      <c r="G24" s="20">
+        <f t="shared" si="3"/>
+        <v>2.4860410853966437</v>
+      </c>
+      <c r="H24" s="20">
+        <f t="shared" si="4"/>
+        <v>1.3446644742821752</v>
+      </c>
+      <c r="I24" s="20">
+        <f t="shared" si="5"/>
+        <v>0.60349027680289336</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
@@ -2855,8 +2912,305 @@
       </c>
       <c r="E26" s="1"/>
     </row>
+    <row r="28" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="35"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G29" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0.275997121711403</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0.43723171579192099</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.67961559318111597</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0.20747440010439</v>
+      </c>
+      <c r="G31" s="20">
+        <f t="shared" ref="G31:G33" si="6">+C31/$B31</f>
+        <v>1.5841894041529654</v>
+      </c>
+      <c r="H31" s="20">
+        <f t="shared" ref="H31:H33" si="7">+D31/$B31</f>
+        <v>2.4624010169633492</v>
+      </c>
+      <c r="I31" s="20">
+        <f t="shared" ref="I31:I33" si="8">+E31/$B31</f>
+        <v>0.75172668040116764</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="9">
+        <v>0.275997121711403</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.53515424366693598</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.55988548385496695</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0.210274263597724</v>
+      </c>
+      <c r="G32" s="20">
+        <f t="shared" si="6"/>
+        <v>1.9389848718296461</v>
+      </c>
+      <c r="H32" s="20">
+        <f t="shared" si="7"/>
+        <v>2.0285917490125582</v>
+      </c>
+      <c r="I32" s="20">
+        <f t="shared" si="8"/>
+        <v>0.76187121914118272</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="23">
+        <v>0.275997121711403</v>
+      </c>
+      <c r="C33" s="23">
+        <v>0.72496424069797205</v>
+      </c>
+      <c r="D33" s="23">
+        <v>0.32478087061987698</v>
+      </c>
+      <c r="E33" s="23">
+        <v>0.210704417602775</v>
+      </c>
+      <c r="G33" s="20">
+        <f t="shared" si="6"/>
+        <v>2.6267094243686806</v>
+      </c>
+      <c r="H33" s="20">
+        <f t="shared" si="7"/>
+        <v>1.1767545567358664</v>
+      </c>
+      <c r="I33" s="20">
+        <f t="shared" si="8"/>
+        <v>0.76342976439840748</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="37" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A37" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="35"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G38" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="9">
+        <v>0.29226548409634201</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0.41674145225074499</v>
+      </c>
+      <c r="D40" s="9">
+        <v>0.68501955449875795</v>
+      </c>
+      <c r="E40" s="9">
+        <v>0.204127957562588</v>
+      </c>
+      <c r="G40" s="20">
+        <f t="shared" ref="G40:G42" si="9">+C40/$B40</f>
+        <v>1.4259003369462913</v>
+      </c>
+      <c r="H40" s="20">
+        <f t="shared" ref="H40:H42" si="10">+D40/$B40</f>
+        <v>2.3438263899576626</v>
+      </c>
+      <c r="I40" s="20">
+        <f t="shared" ref="I40:I42" si="11">+E40/$B40</f>
+        <v>0.69843333773652017</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="9">
+        <v>0.27762799199465299</v>
+      </c>
+      <c r="C41" s="9">
+        <v>0.52044318899345099</v>
+      </c>
+      <c r="D41" s="9">
+        <v>0.55621814522313995</v>
+      </c>
+      <c r="E41" s="9">
+        <v>0.22866707649214199</v>
+      </c>
+      <c r="G41" s="20">
+        <f t="shared" si="9"/>
+        <v>1.8746063221300628</v>
+      </c>
+      <c r="H41" s="20">
+        <f t="shared" si="10"/>
+        <v>2.0034656492197391</v>
+      </c>
+      <c r="I41" s="20">
+        <f t="shared" si="11"/>
+        <v>0.82364560882083548</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="23">
+        <v>0.27345687472769298</v>
+      </c>
+      <c r="C42" s="23">
+        <v>0.70121542720996599</v>
+      </c>
+      <c r="D42" s="23">
+        <v>0.37694277286216099</v>
+      </c>
+      <c r="E42" s="23">
+        <v>0.17042898937228501</v>
+      </c>
+      <c r="G42" s="20">
+        <f t="shared" si="9"/>
+        <v>2.5642632971221984</v>
+      </c>
+      <c r="H42" s="20">
+        <f t="shared" si="10"/>
+        <v>1.3784358986678202</v>
+      </c>
+      <c r="I42" s="20">
+        <f t="shared" si="11"/>
+        <v>0.62323900081867523</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="G29:I29"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A10:E10"/>
@@ -2864,6 +3218,96 @@
     <mergeCell ref="A19:E19"/>
   </mergeCells>
   <conditionalFormatting sqref="G13:G15">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:H15">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:I15">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G6">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H6">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I6">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:G24">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:H24">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:I24">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31:G33">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2873,7 +3317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13:H15">
+  <conditionalFormatting sqref="H31:H33">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2883,7 +3327,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13:I15">
+  <conditionalFormatting sqref="I31:I33">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2893,33 +3337,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G6">
+  <conditionalFormatting sqref="G40:G42">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H6">
+  <conditionalFormatting sqref="H40:H42">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I6">
+  <conditionalFormatting sqref="I40:I42">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
trying to fix my mess
</commit_message>
<xml_diff>
--- a/results/tables/final_tables.xlsx
+++ b/results/tables/final_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAEC78B-737D-4D39-9B32-5ABACB0483A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6119409D-00D7-4DF7-A7F7-A93DFC01FB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="21630" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="summaries" sheetId="4" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="118">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -332,9 +332,6 @@
     <t>Hands</t>
   </si>
   <si>
-    <t>Strenght</t>
-  </si>
-  <si>
     <t>Stamina</t>
   </si>
   <si>
@@ -444,6 +441,57 @@
   </si>
   <si>
     <t>Skill acquisition costs estimates :|</t>
+  </si>
+  <si>
+    <t>Percentiles</t>
+  </si>
+  <si>
+    <t>Smallest</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>Sum of Wgt.</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Largest</t>
+  </si>
+  <si>
+    <t>Std. Dev.</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Freq.</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Cum.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Bad sigma</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Correlation matrix of the whole thing</t>
   </si>
 </sst>
 </file>
@@ -621,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -701,6 +749,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1078,8 +1127,8 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1089,13 +1138,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
       <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1197,12 +1246,12 @@
       <c r="E7" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
@@ -1516,12 +1565,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1723,10 +1772,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4:U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1740,36 +1789,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="41"/>
+      <c r="A1" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
       <c r="AC1" s="35"/>
     </row>
     <row r="2" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1778,69 +1827,69 @@
         <v>63</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>65</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="30"/>
       <c r="G2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="30"/>
       <c r="O2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="T2" s="26"/>
       <c r="U2" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="W2" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="X2" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="X2" s="28" t="s">
+      <c r="Y2" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="Y2" s="28" t="s">
+      <c r="Z2" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="Z2" s="28" t="s">
+      <c r="AA2" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="AA2" s="28" t="s">
+      <c r="AB2" s="28" t="s">
         <v>82</v>
-      </c>
-      <c r="AB2" s="28" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
@@ -1853,7 +1902,7 @@
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
       <c r="F3" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="31">
         <v>1</v>
@@ -1864,7 +1913,7 @@
       <c r="K3" s="31"/>
       <c r="L3" s="31"/>
       <c r="N3" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O3" s="31">
         <v>1</v>
@@ -1873,7 +1922,7 @@
       <c r="Q3" s="31"/>
       <c r="R3" s="31"/>
       <c r="T3" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U3" s="32">
         <v>1</v>
@@ -1888,7 +1937,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="B4" s="31">
         <v>0.51829999999999998</v>
@@ -1898,7 +1947,7 @@
       </c>
       <c r="D4" s="31"/>
       <c r="F4" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="31">
         <v>0.25540000000000002</v>
@@ -1911,7 +1960,7 @@
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
       <c r="N4" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O4" s="31">
         <v>4.3900000000000002E-2</v>
@@ -1922,7 +1971,7 @@
       <c r="Q4" s="31"/>
       <c r="R4" s="31"/>
       <c r="T4" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U4" s="32">
         <v>0.63819999999999999</v>
@@ -1939,7 +1988,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="31">
         <v>0.50839999999999996</v>
@@ -1951,7 +2000,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="31">
         <v>0.28789999999999999</v>
@@ -1966,7 +2015,7 @@
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
       <c r="N5" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O5" s="31">
         <v>0.2888</v>
@@ -1979,7 +2028,7 @@
       </c>
       <c r="R5" s="31"/>
       <c r="T5" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U5" s="32">
         <v>0.21809999999999999</v>
@@ -1998,7 +2047,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="F6" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" s="31">
         <v>0.26</v>
@@ -2015,7 +2064,7 @@
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
       <c r="N6" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O6" s="31">
         <v>0.13589999999999999</v>
@@ -2030,7 +2079,7 @@
         <v>1</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U6" s="32">
         <v>0.30109999999999998</v>
@@ -2051,7 +2100,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="F7" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="31">
         <v>0.35020000000000001</v>
@@ -2070,7 +2119,7 @@
       </c>
       <c r="L7" s="31"/>
       <c r="T7" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U7" s="32">
         <v>0.36630000000000001</v>
@@ -2093,7 +2142,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="F8" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="31">
         <v>0.29680000000000001</v>
@@ -2114,7 +2163,7 @@
         <v>1</v>
       </c>
       <c r="T8" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U8" s="32">
         <v>0.36059999999999998</v>
@@ -2139,7 +2188,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="T9" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U9" s="32">
         <v>0.31609999999999999</v>
@@ -2166,7 +2215,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="T10" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U10" s="32">
         <v>0.48359999999999997</v>
@@ -2191,6 +2240,11 @@
       </c>
       <c r="AB10" s="32">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2219,13 +2273,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2281,16 +2335,16 @@
         <v>HG graduates</v>
       </c>
       <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
         <v>87</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>88</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>89</v>
-      </c>
-      <c r="E6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -2317,16 +2371,16 @@
         <v>College+</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
         <v>91</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>92</v>
-      </c>
-      <c r="E9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -2353,16 +2407,16 @@
         <v>Baseline use</v>
       </c>
       <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
         <v>94</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
         <v>95</v>
-      </c>
-      <c r="D12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -2437,13 +2491,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2463,8 +2517,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2474,21 +2528,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="A1" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2621,21 +2675,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G11" s="44" t="s">
+      <c r="G11" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
@@ -2768,21 +2822,21 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="35"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G20" s="44" t="s">
+      <c r="G20" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
@@ -2908,26 +2962,26 @@
         <v>30</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
+      <c r="A28" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="35"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G29" s="44" t="s">
+      <c r="G29" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
@@ -3053,26 +3107,26 @@
         <v>22</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
+      <c r="A37" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
       <c r="F37" s="35"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="44" t="s">
+      <c r="G38" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3198,10 +3252,10 @@
         <v>22</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3378,14 +3432,216 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="K4" sqref="H4:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="8" max="8" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B2" s="39">
+        <v>0.01</v>
+      </c>
+      <c r="C2">
+        <v>-182.9058</v>
+      </c>
+      <c r="D2">
+        <v>-182.9058</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="C3">
+        <v>-2.4769269999999999</v>
+      </c>
+      <c r="D3">
+        <v>-50.112949999999998</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>81</v>
+      </c>
+      <c r="J3">
+        <v>87.1</v>
+      </c>
+      <c r="K3">
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="C4">
+        <v>-0.61556889999999997</v>
+      </c>
+      <c r="D4">
+        <v>-7.7126910000000004</v>
+      </c>
+      <c r="E4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4">
+        <v>93</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>12.9</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="39">
+        <v>0.25</v>
+      </c>
+      <c r="C5">
+        <v>-0.27974209999999999</v>
+      </c>
+      <c r="D5">
+        <v>-4.6246460000000003</v>
+      </c>
+      <c r="E5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6">
+        <v>93</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>2.5728600000000001E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7">
+        <v>-1.085777</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8">
+        <v>23.465900000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B9" s="39">
+        <v>0.75</v>
+      </c>
+      <c r="C9">
+        <v>0.51879140000000001</v>
+      </c>
+      <c r="D9">
+        <v>2.9860180000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B10" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>1.2561910000000001</v>
+      </c>
+      <c r="D10">
+        <v>4.9187279999999998</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10">
+        <v>550.64859999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B11" s="39">
+        <v>0.95</v>
+      </c>
+      <c r="C11">
+        <v>2.4095110000000002</v>
+      </c>
+      <c r="D11">
+        <v>5.2888260000000002</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11">
+        <v>-3.647764</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B12" s="39">
+        <v>0.99</v>
+      </c>
+      <c r="C12">
+        <v>120.896</v>
+      </c>
+      <c r="D12">
+        <v>120.896</v>
+      </c>
+      <c r="E12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12">
+        <v>47.83531</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Got solutions from the mess
</commit_message>
<xml_diff>
--- a/results/tables/final_tables.xlsx
+++ b/results/tables/final_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2247E66F-9822-4A6D-A0AF-54ED39A5EB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E331E3-A3C4-4809-800B-1045CB509E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21630" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="summaries" sheetId="4" r:id="rId1"/>
@@ -606,7 +606,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +646,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -810,11 +822,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -831,22 +860,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,13 +1409,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1503,12 +1517,12 @@
       <c r="E7" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
@@ -1806,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F3C55B-20D0-4D01-AB90-788A157F68F3}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1909,7 +1923,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="40" t="s">
         <v>118</v>
       </c>
       <c r="B3">
@@ -1917,7 +1931,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="40" t="s">
         <v>116</v>
       </c>
       <c r="B4">
@@ -1928,7 +1942,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="40" t="s">
         <v>64</v>
       </c>
       <c r="B5">
@@ -1942,7 +1956,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="41" t="s">
         <v>75</v>
       </c>
       <c r="B6">
@@ -1959,7 +1973,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="41" t="s">
         <v>76</v>
       </c>
       <c r="B7">
@@ -1979,7 +1993,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="41" t="s">
         <v>119</v>
       </c>
       <c r="B8">
@@ -2002,7 +2016,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="41" t="s">
         <v>120</v>
       </c>
       <c r="B9">
@@ -2028,7 +2042,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="41" t="s">
         <v>121</v>
       </c>
       <c r="B10">
@@ -2057,7 +2071,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="41" t="s">
         <v>122</v>
       </c>
       <c r="B11">
@@ -2089,7 +2103,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="41" t="s">
         <v>81</v>
       </c>
       <c r="B12">
@@ -2124,7 +2138,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="41" t="s">
         <v>123</v>
       </c>
       <c r="B13">
@@ -2162,7 +2176,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="42" t="s">
         <v>124</v>
       </c>
       <c r="B14">
@@ -2203,7 +2217,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="42" t="s">
         <v>66</v>
       </c>
       <c r="B15">
@@ -2247,7 +2261,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="42" t="s">
         <v>67</v>
       </c>
       <c r="B16">
@@ -2294,7 +2308,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="42" t="s">
         <v>125</v>
       </c>
       <c r="B17">
@@ -2344,7 +2358,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="43" t="s">
         <v>126</v>
       </c>
       <c r="B18">
@@ -2397,7 +2411,7 @@
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="43" t="s">
         <v>70</v>
       </c>
       <c r="B19">
@@ -2453,7 +2467,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="43" t="s">
         <v>127</v>
       </c>
       <c r="B20">
@@ -2512,7 +2526,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="43" t="s">
         <v>128</v>
       </c>
       <c r="B21">
@@ -2574,7 +2588,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="43" t="s">
         <v>73</v>
       </c>
       <c r="B22">
@@ -2639,7 +2653,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="43" t="s">
         <v>74</v>
       </c>
       <c r="B23">
@@ -2748,12 +2762,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -2972,36 +2986,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
       <c r="AC1" s="35"/>
     </row>
     <row r="2" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3456,13 +3470,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3674,13 +3688,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3700,8 +3714,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3711,21 +3725,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -3858,21 +3872,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="56"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G11" s="46" t="s">
+      <c r="G11" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
@@ -3905,28 +3919,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="9">
-        <v>0.27885169368546697</v>
+        <v>0.243728048163528</v>
       </c>
       <c r="C13" s="9">
-        <v>0.30320567448449298</v>
+        <v>0.30639338586139098</v>
       </c>
       <c r="D13" s="9">
-        <v>0.233826029968141</v>
+        <v>0.94781940223736805</v>
       </c>
       <c r="E13" s="9">
-        <v>0.91303831241435396</v>
+        <v>6.8997895402579598E-2</v>
       </c>
       <c r="G13" s="20">
         <f t="shared" ref="G13:I15" si="2">+C13/$B13</f>
-        <v>1.087336678781289</v>
+        <v>1.2571117200914768</v>
       </c>
       <c r="H13" s="20">
         <f t="shared" si="2"/>
-        <v>0.83853186214420838</v>
+        <v>3.888840079667129</v>
       </c>
       <c r="I13" s="20">
         <f t="shared" si="2"/>
-        <v>3.2742792426580092</v>
+        <v>0.28309378392217638</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -3934,28 +3948,28 @@
         <v>11</v>
       </c>
       <c r="B14" s="9">
-        <v>0.27885169368546697</v>
+        <v>0.243728048163528</v>
       </c>
       <c r="C14" s="9">
-        <v>0.188967867153742</v>
+        <v>0.649996885772121</v>
       </c>
       <c r="D14" s="9">
-        <v>0.79801410460793898</v>
+        <v>0.62369711452125598</v>
       </c>
       <c r="E14" s="9">
-        <v>0.30461932615272902</v>
+        <v>1.64025266039926E-2</v>
       </c>
       <c r="G14" s="20">
         <f t="shared" si="2"/>
-        <v>0.67766440524793747</v>
+        <v>2.6668940676700825</v>
       </c>
       <c r="H14" s="20">
         <f t="shared" si="2"/>
-        <v>2.8617868303431049</v>
+        <v>2.5589878523246115</v>
       </c>
       <c r="I14" s="20">
         <f t="shared" si="2"/>
-        <v>1.0924062254265052</v>
+        <v>6.7298477658129088E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3963,28 +3977,28 @@
         <v>12</v>
       </c>
       <c r="B15" s="23">
-        <v>0.27885169368546697</v>
+        <v>0.243728048163528</v>
       </c>
       <c r="C15" s="23">
-        <v>0.82120048408405799</v>
+        <v>0.80900159771423297</v>
       </c>
       <c r="D15" s="23">
-        <v>0.190953511290265</v>
+        <v>0.43380470102729102</v>
       </c>
       <c r="E15" s="23">
-        <v>0.25665144370672199</v>
+        <v>1.04049831254575E-2</v>
       </c>
       <c r="G15" s="20">
         <f t="shared" si="2"/>
-        <v>2.9449363323944437</v>
+        <v>3.3192798441131313</v>
       </c>
       <c r="H15" s="20">
         <f t="shared" si="2"/>
-        <v>0.68478519447564323</v>
+        <v>1.7798718871134278</v>
       </c>
       <c r="I15" s="20">
         <f t="shared" si="2"/>
-        <v>0.92038689209545943</v>
+        <v>4.2690954955156957E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -4005,21 +4019,21 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="35"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
@@ -4150,21 +4164,21 @@
       <c r="E26" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="35"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="44"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
@@ -4295,21 +4309,21 @@
       <c r="E35" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="35"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="44"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="46" t="s">
+      <c r="G38" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -4615,10 +4629,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:M12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K4" sqref="H4:K4"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4626,7 +4640,7 @@
     <col min="8" max="8" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>101</v>
       </c>
@@ -4645,8 +4659,9 @@
       <c r="K1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M1" s="44"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2" s="39">
         <v>0.01</v>
       </c>
@@ -4657,7 +4672,7 @@
         <v>-182.9058</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="39">
         <v>0.05</v>
       </c>
@@ -4680,7 +4695,7 @@
         <v>87.1</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="39">
         <v>0.1</v>
       </c>
@@ -4709,7 +4724,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="39">
         <v>0.25</v>
       </c>
@@ -4726,7 +4741,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="H6" t="s">
         <v>114</v>
       </c>
@@ -4737,7 +4752,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7" s="39">
         <v>0.5</v>
       </c>
@@ -4751,7 +4766,7 @@
         <v>-1.085777</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>106</v>
       </c>
@@ -4762,7 +4777,7 @@
         <v>23.465900000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="39">
         <v>0.75</v>
       </c>
@@ -4773,7 +4788,7 @@
         <v>2.9860180000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="39">
         <v>0.9</v>
       </c>
@@ -4790,7 +4805,7 @@
         <v>550.64859999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="39">
         <v>0.95</v>
       </c>
@@ -4807,7 +4822,7 @@
         <v>-3.647764</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" s="39">
         <v>0.99</v>
       </c>

</xml_diff>

<commit_message>
Added two equation to the corection
</commit_message>
<xml_diff>
--- a/results/tables/final_tables.xlsx
+++ b/results/tables/final_tables.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6119409D-00D7-4DF7-A7F7-A93DFC01FB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2A7DE7-F493-4C84-8F72-859A8ED579AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21630" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="summaries" sheetId="4" r:id="rId1"/>
-    <sheet name="top_jobs_skill" sheetId="5" r:id="rId2"/>
-    <sheet name="indexes_make_sense" sheetId="6" r:id="rId3"/>
-    <sheet name="people_do_diff" sheetId="1" r:id="rId4"/>
-    <sheet name="theta_estimates" sheetId="2" r:id="rId5"/>
-    <sheet name="pi_estimates" sheetId="3" r:id="rId6"/>
+    <sheet name="correlation" sheetId="7" r:id="rId2"/>
+    <sheet name="top_jobs_skill" sheetId="5" r:id="rId3"/>
+    <sheet name="indexes_make_sense" sheetId="6" r:id="rId4"/>
+    <sheet name="people_do_diff" sheetId="1" r:id="rId5"/>
+    <sheet name="theta_estimates" sheetId="2" r:id="rId6"/>
+    <sheet name="pi_estimates" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,6 +83,7 @@
     <author>tc={5FB4546E-B91B-4CDE-868E-4F97C041A2D6}</author>
     <author>tc={D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}</author>
     <author>tc={134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}</author>
+    <author>César Garro-Marin</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5FB4546E-B91B-4CDE-868E-4F97C041A2D6}">
@@ -101,7 +103,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="D26" authorId="2" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+    <comment ref="D35" authorId="2" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -109,12 +111,37 @@
     Should I winsorize it?</t>
       </text>
     </comment>
+    <comment ref="F37" authorId="3" shapeId="0" xr:uid="{27F48698-CC06-4FB1-9FD5-2D325DF00A42}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>César Garro-Marin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Already in production
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="129">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -440,9 +467,6 @@
     <t>Skill acquisition costs estimates :)</t>
   </si>
   <si>
-    <t>Skill acquisition costs estimates :|</t>
-  </si>
-  <si>
     <t>Percentiles</t>
   </si>
   <si>
@@ -492,6 +516,42 @@
   </si>
   <si>
     <t>Correlation matrix of the whole thing</t>
+  </si>
+  <si>
+    <t>Hand accuracy</t>
+  </si>
+  <si>
+    <t>Basic math</t>
+  </si>
+  <si>
+    <t>Fractions / percents</t>
+  </si>
+  <si>
+    <t>Advanced math</t>
+  </si>
+  <si>
+    <t>Planning others' time</t>
+  </si>
+  <si>
+    <t>Deep problems</t>
+  </si>
+  <si>
+    <t>Less repetitive</t>
+  </si>
+  <si>
+    <t>Planning my time</t>
+  </si>
+  <si>
+    <t>Dealing with ppl</t>
+  </si>
+  <si>
+    <t>Listening</t>
+  </si>
+  <si>
+    <t>Speeches</t>
+  </si>
+  <si>
+    <t>Same manual</t>
   </si>
 </sst>
 </file>
@@ -503,7 +563,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,8 +623,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,6 +667,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -750,11 +861,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -765,12 +893,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,6 +920,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>3174</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>307490</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>2164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1679B9E5-DB76-32A5-C246-06C1A4F2BFC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4346574"/>
+          <a:ext cx="9451490" cy="6876040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>488949</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>351036</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>126634</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{079E99BD-E5C6-3445-9379-06FE14B56EE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9632949" y="4476750"/>
+          <a:ext cx="5958087" cy="4336684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>332795</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>65665</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{213947F4-548F-C8B8-C445-DE072BBD3D4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10953750"/>
+          <a:ext cx="6428795" cy="4675765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>150991</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>255785</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>20644</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39DEA99B-136C-2412-DB3C-72CEB0482B2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6515099" y="11009491"/>
+          <a:ext cx="6542286" cy="4755978"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1114,7 +1429,7 @@
     <text xml:space="preserve">In production. Panicking a little bit
 </text>
   </threadedComment>
-  <threadedComment ref="D26" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+  <threadedComment ref="D35" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
     <text>Should I winsorize it?</text>
   </threadedComment>
 </ThreadedComments>
@@ -1127,8 +1442,8 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E3:E6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1138,13 +1453,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1246,12 +1561,12 @@
       <c r="E7" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
@@ -1546,6 +1861,932 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F3C55B-20D0-4D01-AB90-788A157F68F3}">
+  <dimension ref="A1:V23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B1" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" t="s">
+        <v>126</v>
+      </c>
+      <c r="T2" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4">
+        <v>0.52429999999999999</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>0.50409999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.75739999999999996</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6">
+        <v>-0.13139999999999999</v>
+      </c>
+      <c r="C6">
+        <v>-0.22650000000000001</v>
+      </c>
+      <c r="D6">
+        <v>-0.14960000000000001</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7">
+        <v>-5.2900000000000003E-2</v>
+      </c>
+      <c r="C7">
+        <v>-0.14449999999999999</v>
+      </c>
+      <c r="D7">
+        <v>-8.3400000000000002E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.66120000000000001</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C8">
+        <v>-8.8099999999999998E-2</v>
+      </c>
+      <c r="D8">
+        <v>-5.8799999999999998E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.23580000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.2475</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9">
+        <v>-1.04E-2</v>
+      </c>
+      <c r="C9">
+        <v>-0.15049999999999999</v>
+      </c>
+      <c r="D9">
+        <v>-0.1196</v>
+      </c>
+      <c r="E9">
+        <v>0.32369999999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.31590000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.75149999999999995</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="C10">
+        <v>-0.11020000000000001</v>
+      </c>
+      <c r="D10">
+        <v>-8.5199999999999998E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.37980000000000003</v>
+      </c>
+      <c r="F10">
+        <v>0.34660000000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.52549999999999997</v>
+      </c>
+      <c r="H10">
+        <v>0.67530000000000001</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="C11">
+        <v>1.11E-2</v>
+      </c>
+      <c r="D11">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.38229999999999997</v>
+      </c>
+      <c r="F11">
+        <v>0.35959999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="H11">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="I11">
+        <v>0.2462</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A12" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12">
+        <v>0.1085</v>
+      </c>
+      <c r="C12">
+        <v>-2.1700000000000001E-2</v>
+      </c>
+      <c r="D12">
+        <v>2.86E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.33560000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="G12">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="H12">
+        <v>0.30640000000000001</v>
+      </c>
+      <c r="I12">
+        <v>0.27229999999999999</v>
+      </c>
+      <c r="J12">
+        <v>0.35289999999999999</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A13" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="C13">
+        <v>-0.1246</v>
+      </c>
+      <c r="D13">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.50249999999999995</v>
+      </c>
+      <c r="F13">
+        <v>0.52749999999999997</v>
+      </c>
+      <c r="G13">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="H13">
+        <v>0.35730000000000001</v>
+      </c>
+      <c r="I13">
+        <v>0.4093</v>
+      </c>
+      <c r="J13">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="K13">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A14" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14">
+        <v>-0.1754</v>
+      </c>
+      <c r="C14">
+        <v>-0.1913</v>
+      </c>
+      <c r="D14">
+        <v>-0.1711</v>
+      </c>
+      <c r="E14">
+        <v>0.161</v>
+      </c>
+      <c r="F14">
+        <v>0.13109999999999999</v>
+      </c>
+      <c r="G14">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="H14">
+        <v>7.6200000000000004E-2</v>
+      </c>
+      <c r="I14">
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="J14">
+        <v>9.5799999999999996E-2</v>
+      </c>
+      <c r="K14">
+        <v>9.9400000000000002E-2</v>
+      </c>
+      <c r="L14">
+        <v>0.15709999999999999</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A15" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C15">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="D15">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.1009</v>
+      </c>
+      <c r="F15">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="G15">
+        <v>7.7299999999999994E-2</v>
+      </c>
+      <c r="H15">
+        <v>7.6200000000000004E-2</v>
+      </c>
+      <c r="I15">
+        <v>5.96E-2</v>
+      </c>
+      <c r="J15">
+        <v>0.15659999999999999</v>
+      </c>
+      <c r="K15">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="L15">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="M15">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A16" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16">
+        <v>-3.5099999999999999E-2</v>
+      </c>
+      <c r="C16">
+        <v>-0.1091</v>
+      </c>
+      <c r="D16">
+        <v>-5.5199999999999999E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.29409999999999997</v>
+      </c>
+      <c r="F16">
+        <v>0.2853</v>
+      </c>
+      <c r="G16">
+        <v>0.16639999999999999</v>
+      </c>
+      <c r="H16">
+        <v>0.1991</v>
+      </c>
+      <c r="I16">
+        <v>0.16930000000000001</v>
+      </c>
+      <c r="J16">
+        <v>0.27360000000000001</v>
+      </c>
+      <c r="K16">
+        <v>0.29730000000000001</v>
+      </c>
+      <c r="L16">
+        <v>0.31590000000000001</v>
+      </c>
+      <c r="M16">
+        <v>0.30869999999999997</v>
+      </c>
+      <c r="N16">
+        <v>0.22389999999999999</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A17" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17">
+        <v>-6.2399999999999997E-2</v>
+      </c>
+      <c r="C17">
+        <v>-0.11509999999999999</v>
+      </c>
+      <c r="D17">
+        <v>-3.7199999999999997E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.377</v>
+      </c>
+      <c r="F17">
+        <v>0.3533</v>
+      </c>
+      <c r="G17">
+        <v>0.23119999999999999</v>
+      </c>
+      <c r="H17">
+        <v>0.2641</v>
+      </c>
+      <c r="I17">
+        <v>0.21110000000000001</v>
+      </c>
+      <c r="J17">
+        <v>0.44019999999999998</v>
+      </c>
+      <c r="K17">
+        <v>0.3957</v>
+      </c>
+      <c r="L17">
+        <v>0.39829999999999999</v>
+      </c>
+      <c r="M17">
+        <v>0.155</v>
+      </c>
+      <c r="N17">
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="O17">
+        <v>0.34210000000000002</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A18" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18">
+        <v>-0.10829999999999999</v>
+      </c>
+      <c r="C18">
+        <v>-9.69E-2</v>
+      </c>
+      <c r="D18">
+        <v>-2.7699999999999999E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="F18">
+        <v>0.2676</v>
+      </c>
+      <c r="G18">
+        <v>0.1384</v>
+      </c>
+      <c r="H18">
+        <v>0.1226</v>
+      </c>
+      <c r="I18">
+        <v>7.0599999999999996E-2</v>
+      </c>
+      <c r="J18">
+        <v>0.25750000000000001</v>
+      </c>
+      <c r="K18">
+        <v>0.21529999999999999</v>
+      </c>
+      <c r="L18">
+        <v>0.2135</v>
+      </c>
+      <c r="M18">
+        <v>8.8499999999999995E-2</v>
+      </c>
+      <c r="N18">
+        <v>0.13289999999999999</v>
+      </c>
+      <c r="O18">
+        <v>0.27060000000000001</v>
+      </c>
+      <c r="P18">
+        <v>0.2878</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A19" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19">
+        <v>-8.0999999999999996E-3</v>
+      </c>
+      <c r="C19">
+        <v>-8.8999999999999999E-3</v>
+      </c>
+      <c r="D19">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="F19">
+        <v>0.27789999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.1031</v>
+      </c>
+      <c r="H19">
+        <v>0.1129</v>
+      </c>
+      <c r="I19">
+        <v>0.1187</v>
+      </c>
+      <c r="J19">
+        <v>0.35909999999999997</v>
+      </c>
+      <c r="K19">
+        <v>0.23769999999999999</v>
+      </c>
+      <c r="L19">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="M19">
+        <v>-1.03E-2</v>
+      </c>
+      <c r="N19">
+        <v>-5.5999999999999999E-3</v>
+      </c>
+      <c r="O19">
+        <v>0.15260000000000001</v>
+      </c>
+      <c r="P19">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="Q19">
+        <v>0.2596</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A20" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20">
+        <v>-1.83E-2</v>
+      </c>
+      <c r="C20">
+        <v>-5.3600000000000002E-2</v>
+      </c>
+      <c r="D20">
+        <v>-4.8999999999999998E-3</v>
+      </c>
+      <c r="E20">
+        <v>0.30520000000000003</v>
+      </c>
+      <c r="F20">
+        <v>0.34379999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.13650000000000001</v>
+      </c>
+      <c r="H20">
+        <v>0.15060000000000001</v>
+      </c>
+      <c r="I20">
+        <v>0.15359999999999999</v>
+      </c>
+      <c r="J20">
+        <v>0.33860000000000001</v>
+      </c>
+      <c r="K20">
+        <v>0.2984</v>
+      </c>
+      <c r="L20">
+        <v>0.30840000000000001</v>
+      </c>
+      <c r="M20">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="N20">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="O20">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="P20">
+        <v>0.21129999999999999</v>
+      </c>
+      <c r="Q20">
+        <v>0.29580000000000001</v>
+      </c>
+      <c r="R20">
+        <v>0.64780000000000004</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A21" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21">
+        <v>-0.16220000000000001</v>
+      </c>
+      <c r="C21">
+        <v>-0.20030000000000001</v>
+      </c>
+      <c r="D21">
+        <v>-0.1011</v>
+      </c>
+      <c r="E21">
+        <v>0.51729999999999998</v>
+      </c>
+      <c r="F21">
+        <v>0.43959999999999999</v>
+      </c>
+      <c r="G21">
+        <v>0.16980000000000001</v>
+      </c>
+      <c r="H21">
+        <v>0.25819999999999999</v>
+      </c>
+      <c r="I21">
+        <v>0.29730000000000001</v>
+      </c>
+      <c r="J21">
+        <v>0.42649999999999999</v>
+      </c>
+      <c r="K21">
+        <v>0.2888</v>
+      </c>
+      <c r="L21">
+        <v>0.43159999999999998</v>
+      </c>
+      <c r="M21">
+        <v>0.21290000000000001</v>
+      </c>
+      <c r="N21">
+        <v>8.1600000000000006E-2</v>
+      </c>
+      <c r="O21">
+        <v>0.29630000000000001</v>
+      </c>
+      <c r="P21">
+        <v>0.36470000000000002</v>
+      </c>
+      <c r="Q21">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="R21">
+        <v>0.2651</v>
+      </c>
+      <c r="S21">
+        <v>0.27389999999999998</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A22" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22">
+        <v>-0.12180000000000001</v>
+      </c>
+      <c r="C22">
+        <v>-0.14349999999999999</v>
+      </c>
+      <c r="D22">
+        <v>-4.7600000000000003E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="F22">
+        <v>0.41420000000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.20979999999999999</v>
+      </c>
+      <c r="H22">
+        <v>0.26329999999999998</v>
+      </c>
+      <c r="I22">
+        <v>0.24579999999999999</v>
+      </c>
+      <c r="J22">
+        <v>0.48089999999999999</v>
+      </c>
+      <c r="K22">
+        <v>0.3851</v>
+      </c>
+      <c r="L22">
+        <v>0.45639999999999997</v>
+      </c>
+      <c r="M22">
+        <v>0.1653</v>
+      </c>
+      <c r="N22">
+        <v>0.1512</v>
+      </c>
+      <c r="O22">
+        <v>0.31830000000000003</v>
+      </c>
+      <c r="P22">
+        <v>0.3967</v>
+      </c>
+      <c r="Q22">
+        <v>0.37580000000000002</v>
+      </c>
+      <c r="R22">
+        <v>0.31369999999999998</v>
+      </c>
+      <c r="S22">
+        <v>0.33760000000000001</v>
+      </c>
+      <c r="T22">
+        <v>0.59350000000000003</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A23" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23">
+        <v>2.93E-2</v>
+      </c>
+      <c r="C23">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="D23">
+        <v>7.3400000000000007E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.32490000000000002</v>
+      </c>
+      <c r="F23">
+        <v>0.36280000000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.15340000000000001</v>
+      </c>
+      <c r="H23">
+        <v>0.1782</v>
+      </c>
+      <c r="I23">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="J23">
+        <v>0.51160000000000005</v>
+      </c>
+      <c r="K23">
+        <v>0.33250000000000002</v>
+      </c>
+      <c r="L23">
+        <v>0.35649999999999998</v>
+      </c>
+      <c r="M23">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="N23">
+        <v>8.6800000000000002E-2</v>
+      </c>
+      <c r="O23">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="P23">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="Q23">
+        <v>0.31819999999999998</v>
+      </c>
+      <c r="R23">
+        <v>0.42980000000000002</v>
+      </c>
+      <c r="S23">
+        <v>0.40849999999999997</v>
+      </c>
+      <c r="T23">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="U23">
+        <v>0.47870000000000001</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:V1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:V23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1118EAC5-EE01-4F6F-831E-9781C531891C}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -1565,12 +2806,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1767,7 +3008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FC4A17-C099-4E4B-9183-D165FAAEB730}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
@@ -1789,36 +3030,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
       <c r="AC1" s="35"/>
     </row>
     <row r="2" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1827,7 +3068,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>64</v>
@@ -1937,7 +3178,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="31">
         <v>0.51829999999999998</v>
@@ -2244,7 +3485,7 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2255,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070238CE-FD1A-4190-90A2-45E1D7B1D1C6}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -2273,13 +3514,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2491,13 +3732,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2510,15 +3751,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A63E760-C2E1-4C8F-8338-4A55E5F2D8F6}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2528,21 +3769,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2574,87 +3815,63 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9">
-        <v>0.24072823758123699</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0.36823580676442402</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0.767879233440253</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0.21333003904938899</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="G4" s="20" t="e">
         <f>+C4/$B4</f>
-        <v>1.529674335110595</v>
-      </c>
-      <c r="H4" s="20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" s="20" t="e">
         <f t="shared" ref="H4:I6" si="0">+D4/$B4</f>
-        <v>3.1898178674660955</v>
-      </c>
-      <c r="I4" s="20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4" s="20" t="e">
         <f t="shared" si="0"/>
-        <v>0.88618618734911769</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9">
-        <v>0.24072823758123699</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.19519018525746901</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.64705534179666802</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0.53952349185391701</v>
-      </c>
-      <c r="G5" s="20">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="G5" s="20" t="e">
         <f t="shared" ref="G5:G6" si="1">+C5/$B5</f>
-        <v>0.8108321118398063</v>
-      </c>
-      <c r="H5" s="20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="20" t="e">
         <f t="shared" si="0"/>
-        <v>2.6879079425749151</v>
-      </c>
-      <c r="I5" s="20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" s="20" t="e">
         <f t="shared" si="0"/>
-        <v>2.2412139816869119</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="23">
-        <v>0.24072823758123699</v>
-      </c>
-      <c r="C6" s="23">
-        <v>0.72144995745774898</v>
-      </c>
-      <c r="D6" s="23">
-        <v>0.43889801398964001</v>
-      </c>
-      <c r="E6" s="23">
-        <v>0.11339157652500501</v>
-      </c>
-      <c r="G6" s="20">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="G6" s="20" t="e">
         <f t="shared" si="1"/>
-        <v>2.9969477810607321</v>
-      </c>
-      <c r="H6" s="20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="20" t="e">
         <f t="shared" si="0"/>
-        <v>1.8232095179175978</v>
-      </c>
-      <c r="I6" s="20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" s="20" t="e">
         <f t="shared" si="0"/>
-        <v>0.47103562782799624</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2675,21 +3892,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="56"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G11" s="45" t="s">
+      <c r="G11" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
@@ -2722,28 +3939,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="9">
-        <v>0.27885169368546697</v>
+        <v>0.243728048163528</v>
       </c>
       <c r="C13" s="9">
-        <v>0.30320567448449298</v>
+        <v>0.30639338586139098</v>
       </c>
       <c r="D13" s="9">
-        <v>0.233826029968141</v>
+        <v>0.94781940223736805</v>
       </c>
       <c r="E13" s="9">
-        <v>0.91303831241435396</v>
+        <v>6.8997895402579598E-2</v>
       </c>
       <c r="G13" s="20">
         <f t="shared" ref="G13:I15" si="2">+C13/$B13</f>
-        <v>1.087336678781289</v>
+        <v>1.2571117200914768</v>
       </c>
       <c r="H13" s="20">
         <f t="shared" si="2"/>
-        <v>0.83853186214420838</v>
+        <v>3.888840079667129</v>
       </c>
       <c r="I13" s="20">
         <f t="shared" si="2"/>
-        <v>3.2742792426580092</v>
+        <v>0.28309378392217638</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2751,28 +3968,28 @@
         <v>11</v>
       </c>
       <c r="B14" s="9">
-        <v>0.27885169368546697</v>
+        <v>0.243728048163528</v>
       </c>
       <c r="C14" s="9">
-        <v>0.188967867153742</v>
+        <v>0.649996885772121</v>
       </c>
       <c r="D14" s="9">
-        <v>0.79801410460793898</v>
+        <v>0.62369711452125598</v>
       </c>
       <c r="E14" s="9">
-        <v>0.30461932615272902</v>
+        <v>1.64025266039926E-2</v>
       </c>
       <c r="G14" s="20">
         <f t="shared" si="2"/>
-        <v>0.67766440524793747</v>
+        <v>2.6668940676700825</v>
       </c>
       <c r="H14" s="20">
         <f t="shared" si="2"/>
-        <v>2.8617868303431049</v>
+        <v>2.5589878523246115</v>
       </c>
       <c r="I14" s="20">
         <f t="shared" si="2"/>
-        <v>1.0924062254265052</v>
+        <v>6.7298477658129088E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2780,28 +3997,28 @@
         <v>12</v>
       </c>
       <c r="B15" s="23">
-        <v>0.27885169368546697</v>
+        <v>0.243728048163528</v>
       </c>
       <c r="C15" s="23">
-        <v>0.82120048408405799</v>
+        <v>0.80900159771423297</v>
       </c>
       <c r="D15" s="23">
-        <v>0.190953511290265</v>
+        <v>0.43380470102729102</v>
       </c>
       <c r="E15" s="23">
-        <v>0.25665144370672199</v>
+        <v>1.04049831254575E-2</v>
       </c>
       <c r="G15" s="20">
         <f t="shared" si="2"/>
-        <v>2.9449363323944437</v>
+        <v>3.3192798441131313</v>
       </c>
       <c r="H15" s="20">
         <f t="shared" si="2"/>
-        <v>0.68478519447564323</v>
+        <v>1.7798718871134278</v>
       </c>
       <c r="I15" s="20">
         <f t="shared" si="2"/>
-        <v>0.92038689209545943</v>
+        <v>4.2690954955156957E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -2822,21 +4039,21 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="35"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="56"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
@@ -2869,28 +4086,28 @@
         <v>10</v>
       </c>
       <c r="B22" s="9">
-        <v>0.28041979658886301</v>
+        <v>0.28653203408786099</v>
       </c>
       <c r="C22" s="9">
-        <v>0.41399915754056499</v>
+        <v>0.432813593737364</v>
       </c>
       <c r="D22" s="9">
-        <v>0.69763918662608104</v>
+        <v>0.72863646579924202</v>
       </c>
       <c r="E22" s="9">
-        <v>0.20209181959310901</v>
+        <v>0.13590170492659701</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" ref="G22:G24" si="3">+C22/$B22</f>
-        <v>1.476354959873069</v>
+        <f>+C22/$B22</f>
+        <v>1.5105242773820111</v>
       </c>
       <c r="H22" s="20">
-        <f t="shared" ref="H22:H24" si="4">+D22/$B22</f>
-        <v>2.4878385731408383</v>
+        <f>+D22/$B22</f>
+        <v>2.5429494057052482</v>
       </c>
       <c r="I22" s="20">
-        <f t="shared" ref="I22:I24" si="5">+E22/$B22</f>
-        <v>0.72067600808300125</v>
+        <f>+E22/$B22</f>
+        <v>0.47429846843904605</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -2898,28 +4115,28 @@
         <v>11</v>
       </c>
       <c r="B23" s="9">
-        <v>0.28041979658886301</v>
+        <v>0.276932075864669</v>
       </c>
       <c r="C23" s="9">
-        <v>0.52861914399065901</v>
+        <v>0.57770093297611302</v>
       </c>
       <c r="D23" s="9">
-        <v>0.55762567138944696</v>
+        <v>0.59045981810458203</v>
       </c>
       <c r="E23" s="9">
-        <v>0.21526761088893601</v>
+        <v>0.11649908855437099</v>
       </c>
       <c r="G23" s="20">
-        <f t="shared" si="3"/>
-        <v>1.88509923486498</v>
+        <f>+C23/$B23</f>
+        <v>2.0860744685221064</v>
       </c>
       <c r="H23" s="20">
-        <f t="shared" si="4"/>
-        <v>1.9885388912360167</v>
+        <f>+D23/$B23</f>
+        <v>2.1321467232027236</v>
       </c>
       <c r="I23" s="20">
-        <f t="shared" si="5"/>
-        <v>0.76766196077287019</v>
+        <f>+E23/$B23</f>
+        <v>0.42067748270265992</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2927,28 +4144,28 @@
         <v>12</v>
       </c>
       <c r="B24" s="23">
-        <v>0.28041979658886301</v>
+        <v>0.26284326769114302</v>
       </c>
       <c r="C24" s="23">
-        <v>0.69713513547848305</v>
+        <v>0.69281313851899595</v>
       </c>
       <c r="D24" s="23">
-        <v>0.37707053835847798</v>
+        <v>0.46538756699114298</v>
       </c>
       <c r="E24" s="23">
-        <v>0.16923062066442399</v>
+        <v>8.4193690103555402E-2</v>
       </c>
       <c r="G24" s="20">
-        <f t="shared" si="3"/>
-        <v>2.4860410853966437</v>
+        <f>+C24/$B24</f>
+        <v>2.635841292815968</v>
       </c>
       <c r="H24" s="20">
-        <f t="shared" si="4"/>
-        <v>1.3446644742821752</v>
+        <f>+D24/$B24</f>
+        <v>1.7705896410403859</v>
       </c>
       <c r="I24" s="20">
-        <f t="shared" si="5"/>
-        <v>0.60349027680289336</v>
+        <f>+E24/$B24</f>
+        <v>0.32031899026034083</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -2964,24 +4181,33 @@
       <c r="D26" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="57"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
     </row>
     <row r="28" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="35"/>
+      <c r="A28" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="44"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G29" s="45" t="s">
+      <c r="G29" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
@@ -3013,87 +4239,63 @@
       <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="9">
-        <v>0.275997121711403</v>
-      </c>
-      <c r="C31" s="9">
-        <v>0.43723171579192099</v>
-      </c>
-      <c r="D31" s="9">
-        <v>0.67961559318111597</v>
-      </c>
-      <c r="E31" s="9">
-        <v>0.20747440010439</v>
-      </c>
-      <c r="G31" s="20">
-        <f t="shared" ref="G31:G33" si="6">+C31/$B31</f>
-        <v>1.5841894041529654</v>
-      </c>
-      <c r="H31" s="20">
-        <f t="shared" ref="H31:H33" si="7">+D31/$B31</f>
-        <v>2.4624010169633492</v>
-      </c>
-      <c r="I31" s="20">
-        <f t="shared" ref="I31:I33" si="8">+E31/$B31</f>
-        <v>0.75172668040116764</v>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="G31" s="20" t="e">
+        <f t="shared" ref="G31:G33" si="3">+C31/$B31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="20" t="e">
+        <f t="shared" ref="H31:H33" si="4">+D31/$B31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="20" t="e">
+        <f t="shared" ref="I31:I33" si="5">+E31/$B31</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="9">
-        <v>0.275997121711403</v>
-      </c>
-      <c r="C32" s="9">
-        <v>0.53515424366693598</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0.55988548385496695</v>
-      </c>
-      <c r="E32" s="9">
-        <v>0.210274263597724</v>
-      </c>
-      <c r="G32" s="20">
-        <f t="shared" si="6"/>
-        <v>1.9389848718296461</v>
-      </c>
-      <c r="H32" s="20">
-        <f t="shared" si="7"/>
-        <v>2.0285917490125582</v>
-      </c>
-      <c r="I32" s="20">
-        <f t="shared" si="8"/>
-        <v>0.76187121914118272</v>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="G32" s="20" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="23">
-        <v>0.275997121711403</v>
-      </c>
-      <c r="C33" s="23">
-        <v>0.72496424069797205</v>
-      </c>
-      <c r="D33" s="23">
-        <v>0.32478087061987698</v>
-      </c>
-      <c r="E33" s="23">
-        <v>0.210704417602775</v>
-      </c>
-      <c r="G33" s="20">
-        <f t="shared" si="6"/>
-        <v>2.6267094243686806</v>
-      </c>
-      <c r="H33" s="20">
-        <f t="shared" si="7"/>
-        <v>1.1767545567358664</v>
-      </c>
-      <c r="I33" s="20">
-        <f t="shared" si="8"/>
-        <v>0.76342976439840748</v>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="G33" s="20" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -3104,29 +4306,31 @@
         <v>29</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="24" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="35"/>
+      <c r="A37" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="44"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="45" t="s">
+      <c r="G38" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3158,87 +4362,63 @@
       <c r="A40" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="9">
-        <v>0.29226548409634201</v>
-      </c>
-      <c r="C40" s="9">
-        <v>0.41674145225074499</v>
-      </c>
-      <c r="D40" s="9">
-        <v>0.68501955449875795</v>
-      </c>
-      <c r="E40" s="9">
-        <v>0.204127957562588</v>
-      </c>
-      <c r="G40" s="20">
-        <f t="shared" ref="G40:G42" si="9">+C40/$B40</f>
-        <v>1.4259003369462913</v>
-      </c>
-      <c r="H40" s="20">
-        <f t="shared" ref="H40:H42" si="10">+D40/$B40</f>
-        <v>2.3438263899576626</v>
-      </c>
-      <c r="I40" s="20">
-        <f t="shared" ref="I40:I42" si="11">+E40/$B40</f>
-        <v>0.69843333773652017</v>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="G40" s="20" t="e">
+        <f t="shared" ref="G40:G42" si="6">+C40/$B40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="20" t="e">
+        <f t="shared" ref="H40:H42" si="7">+D40/$B40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" s="20" t="e">
+        <f t="shared" ref="I40:I42" si="8">+E40/$B40</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="9">
-        <v>0.27762799199465299</v>
-      </c>
-      <c r="C41" s="9">
-        <v>0.52044318899345099</v>
-      </c>
-      <c r="D41" s="9">
-        <v>0.55621814522313995</v>
-      </c>
-      <c r="E41" s="9">
-        <v>0.22866707649214199</v>
-      </c>
-      <c r="G41" s="20">
-        <f t="shared" si="9"/>
-        <v>1.8746063221300628</v>
-      </c>
-      <c r="H41" s="20">
-        <f t="shared" si="10"/>
-        <v>2.0034656492197391</v>
-      </c>
-      <c r="I41" s="20">
-        <f t="shared" si="11"/>
-        <v>0.82364560882083548</v>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="G41" s="20" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" s="20" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" s="20" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="23">
-        <v>0.27345687472769298</v>
-      </c>
-      <c r="C42" s="23">
-        <v>0.70121542720996599</v>
-      </c>
-      <c r="D42" s="23">
-        <v>0.37694277286216099</v>
-      </c>
-      <c r="E42" s="23">
-        <v>0.17042898937228501</v>
-      </c>
-      <c r="G42" s="20">
-        <f t="shared" si="9"/>
-        <v>2.5642632971221984</v>
-      </c>
-      <c r="H42" s="20">
-        <f t="shared" si="10"/>
-        <v>1.3784358986678202</v>
-      </c>
-      <c r="I42" s="20">
-        <f t="shared" si="11"/>
-        <v>0.62323900081867523</v>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="G42" s="20" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H42" s="20" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" s="20" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -3255,21 +4435,21 @@
         <v>96</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="G29:I29"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="A28:E28"/>
     <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="G38:I38"/>
   </mergeCells>
   <conditionalFormatting sqref="G13:G15">
     <cfRule type="colorScale" priority="15">
@@ -3331,7 +4511,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22:G24">
+  <conditionalFormatting sqref="G31:G33">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3341,7 +4521,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22:H24">
+  <conditionalFormatting sqref="H31:H33">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3351,7 +4531,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:I24">
+  <conditionalFormatting sqref="I31:I33">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3361,7 +4541,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G31:G33">
+  <conditionalFormatting sqref="G40:G42">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3371,7 +4551,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31:H33">
+  <conditionalFormatting sqref="H40:H42">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3381,7 +4561,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31:I33">
+  <conditionalFormatting sqref="I40:I42">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3391,7 +4571,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40:G42">
+  <conditionalFormatting sqref="G22:G24">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3401,7 +4581,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40:H42">
+  <conditionalFormatting sqref="H22:H24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3411,7 +4591,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40:I42">
+  <conditionalFormatting sqref="I22:I24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3427,15 +4607,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C324394-3725-49AA-88D9-CE062D28E523}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:M12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K4" sqref="H4:K4"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3443,27 +4623,28 @@
     <col min="8" max="8" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
-        <v>102</v>
-      </c>
       <c r="H1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" t="s">
         <v>111</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>112</v>
       </c>
-      <c r="K1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M1" s="44"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2" s="39">
         <v>0.01</v>
       </c>
@@ -3474,7 +4655,7 @@
         <v>-182.9058</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="39">
         <v>0.05</v>
       </c>
@@ -3497,7 +4678,7 @@
         <v>87.1</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="39">
         <v>0.1</v>
       </c>
@@ -3508,7 +4689,7 @@
         <v>-7.7126910000000004</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4">
         <v>93</v>
@@ -3526,7 +4707,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="39">
         <v>0.25</v>
       </c>
@@ -3537,15 +4718,15 @@
         <v>-4.6246460000000003</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F5">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="H6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I6">
         <v>93</v>
@@ -3554,7 +4735,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7" s="39">
         <v>0.5</v>
       </c>
@@ -3562,24 +4743,24 @@
         <v>2.5728600000000001E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7">
         <v>-1.085777</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" t="s">
         <v>106</v>
-      </c>
-      <c r="E8" t="s">
-        <v>107</v>
       </c>
       <c r="F8">
         <v>23.465900000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="39">
         <v>0.75</v>
       </c>
@@ -3590,7 +4771,7 @@
         <v>2.9860180000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="39">
         <v>0.9</v>
       </c>
@@ -3601,13 +4782,13 @@
         <v>4.9187279999999998</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10">
         <v>550.64859999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="39">
         <v>0.95</v>
       </c>
@@ -3618,13 +4799,13 @@
         <v>5.2888260000000002</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F11">
         <v>-3.647764</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" s="39">
         <v>0.99</v>
       </c>
@@ -3635,7 +4816,7 @@
         <v>120.896</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F12">
         <v>47.83531</v>

</xml_diff>

<commit_message>
Finished fixing all the mistakes
</commit_message>
<xml_diff>
--- a/results/tables/final_tables.xlsx
+++ b/results/tables/final_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE3B13C-84BA-4B93-B96B-8E6D534A643B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D432F-04EB-408D-BFD0-D8A5C7708DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="theta_estimates" sheetId="2" r:id="rId1"/>
@@ -45,60 +45,15 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={5FB4546E-B91B-4CDE-868E-4F97C041A2D6}</author>
-    <author>tc={D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}</author>
     <author>tc={134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}</author>
-    <author>César Garro-Marin</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5FB4546E-B91B-4CDE-868E-4F97C041A2D6}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    I have to correct this. I just realized a variable had the wrong sign</t>
-      </text>
-    </comment>
-    <comment ref="A10" authorId="1" shapeId="0" xr:uid="{D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    In production. Panicking a little bit
-</t>
-      </text>
-    </comment>
-    <comment ref="D35" authorId="2" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Should I winsorize it?</t>
-      </text>
-    </comment>
-    <comment ref="F37" authorId="3" shapeId="0" xr:uid="{27F48698-CC06-4FB1-9FD5-2D325DF00A42}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>César Garro-Marin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Already in production
-</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -160,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="127">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -480,9 +435,6 @@
     <t>Different manual</t>
   </si>
   <si>
-    <t>Skill acquisition costs estimates :)</t>
-  </si>
-  <si>
     <t>Percentiles</t>
   </si>
   <si>
@@ -514,12 +466,6 @@
   </si>
   <si>
     <t>Freq.</t>
-  </si>
-  <si>
-    <t>Percent</t>
-  </si>
-  <si>
-    <t>Cum.</t>
   </si>
   <si>
     <t>Total</t>
@@ -585,7 +531,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -652,19 +598,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -889,6 +822,12 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -915,12 +854,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1423,13 +1356,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2023-05-04T14:24:46.91" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{5FB4546E-B91B-4CDE-868E-4F97C041A2D6}" done="1">
-    <text>I have to correct this. I just realized a variable had the wrong sign</text>
-  </threadedComment>
-  <threadedComment ref="A10" dT="2023-05-05T16:03:41.57" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{D6BE0F47-99D2-4C68-A48E-D56E8CAB5FF3}">
-    <text xml:space="preserve">In production. Panicking a little bit
-</text>
-  </threadedComment>
   <threadedComment ref="D35" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
     <text>Should I winsorize it?</text>
   </threadedComment>
@@ -1467,8 +1393,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A27" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E10"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1478,24 +1404,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -1628,21 +1554,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
@@ -1775,21 +1701,21 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
       <c r="F19" s="45"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G20" s="55" t="s">
+      <c r="G20" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
@@ -1929,21 +1855,21 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
       <c r="F28" s="45"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G29" s="55" t="s">
+      <c r="G29" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
@@ -2072,25 +1998,25 @@
         <v>96</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
+      <c r="A37" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
       <c r="F37" s="45"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="55" t="s">
+      <c r="G38" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -2219,7 +2145,7 @@
         <v>96</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2398,8 +2324,8 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2409,24 +2335,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2459,28 +2385,28 @@
         <v>10</v>
       </c>
       <c r="B4" s="9">
-        <v>0.244299027114214</v>
+        <v>0.29593120000000001</v>
       </c>
       <c r="C4" s="9">
-        <v>0.284013423333426</v>
+        <v>0.43839400000000001</v>
       </c>
       <c r="D4" s="9">
-        <v>0.81678328589676596</v>
+        <v>0.67276720000000001</v>
       </c>
       <c r="E4" s="9">
-        <v>0.246151527775374</v>
+        <v>0.1945896</v>
       </c>
       <c r="G4" s="20">
         <f>+C4/$B4</f>
-        <v>1.1625646924932076</v>
+        <v>1.481405137410317</v>
       </c>
       <c r="H4" s="20">
         <f t="shared" ref="H4:I6" si="0">+D4/$B4</f>
-        <v>3.3433751069131592</v>
+        <v>2.2733905718626493</v>
       </c>
       <c r="I4" s="20">
         <f t="shared" si="0"/>
-        <v>1.0075829227936053</v>
+        <v>0.65755013327422052</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -2488,28 +2414,28 @@
         <v>11</v>
       </c>
       <c r="B5" s="9">
-        <v>0.244299027114214</v>
+        <v>0.27454250000000002</v>
       </c>
       <c r="C5" s="9">
-        <v>0.39134666027288501</v>
+        <v>0.5662315</v>
       </c>
       <c r="D5" s="9">
-        <v>0.84550065690207798</v>
+        <v>0.65564169999999999</v>
       </c>
       <c r="E5" s="9">
-        <v>2.68823275696158E-2</v>
+        <v>5.9034499999999997E-2</v>
       </c>
       <c r="G5" s="20">
         <f t="shared" ref="G5:G6" si="1">+C5/$B5</f>
-        <v>1.6019165728806759</v>
+        <v>2.0624548111858818</v>
       </c>
       <c r="H5" s="20">
         <f t="shared" si="0"/>
-        <v>3.4609251902865412</v>
+        <v>2.3881246073012372</v>
       </c>
       <c r="I5" s="20">
         <f t="shared" si="0"/>
-        <v>0.1100386190119695</v>
+        <v>0.21502863855322943</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2517,28 +2443,28 @@
         <v>12</v>
       </c>
       <c r="B6" s="23">
-        <v>0.244299027114214</v>
+        <v>0.27069300000000002</v>
       </c>
       <c r="C6" s="23">
-        <v>0.98766734287929203</v>
+        <v>0.62212940000000005</v>
       </c>
       <c r="D6" s="23">
-        <v>0.17820408513814101</v>
+        <v>0.54990119999999998</v>
       </c>
       <c r="E6" s="23">
-        <v>0.101593597684959</v>
+        <v>7.5414999999999996E-2</v>
       </c>
       <c r="G6" s="20">
         <f t="shared" si="1"/>
-        <v>4.0428623664454486</v>
+        <v>2.2982840339425108</v>
       </c>
       <c r="H6" s="20">
         <f t="shared" si="0"/>
-        <v>0.72945065415601318</v>
+        <v>2.0314570380467907</v>
       </c>
       <c r="I6" s="20">
         <f t="shared" si="0"/>
-        <v>0.41585756146897074</v>
+        <v>0.27859974214331362</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2546,7 +2472,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>24</v>
@@ -2600,10 +2526,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B1:M12"/>
+  <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2611,73 +2537,61 @@
     <col min="8" max="8" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
-        <v>100</v>
-      </c>
       <c r="H1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J1" t="s">
-        <v>110</v>
-      </c>
-      <c r="K1" t="s">
-        <v>111</v>
-      </c>
-      <c r="M1" s="44"/>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+      <c r="K1" s="45"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2" s="39">
         <v>0.01</v>
       </c>
       <c r="C2">
-        <v>-182.9058</v>
+        <v>-80.663570000000007</v>
       </c>
       <c r="D2">
-        <v>-182.9058</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+        <v>-80.663570000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="39">
         <v>0.05</v>
       </c>
       <c r="C3">
-        <v>-2.4769269999999999</v>
+        <v>-4.4692429999999996</v>
       </c>
       <c r="D3">
-        <v>-50.112949999999998</v>
+        <v>-14.09618</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>81</v>
-      </c>
-      <c r="J3">
-        <v>87.1</v>
-      </c>
-      <c r="K3">
-        <v>87.1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="39">
         <v>0.1</v>
       </c>
       <c r="C4">
-        <v>-0.61556889999999997</v>
+        <v>-0.73104380000000002</v>
       </c>
       <c r="D4">
-        <v>-7.7126910000000004</v>
+        <v>-11.94042</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4">
         <v>93</v>
@@ -2686,128 +2600,119 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>12</v>
-      </c>
-      <c r="J4">
-        <v>12.9</v>
-      </c>
-      <c r="K4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="39">
         <v>0.25</v>
       </c>
       <c r="C5">
-        <v>-0.27974209999999999</v>
+        <v>-0.25560250000000001</v>
       </c>
       <c r="D5">
-        <v>-4.6246460000000003</v>
+        <v>-5.2036160000000002</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="H6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I6">
         <v>93</v>
       </c>
-      <c r="J6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="39">
         <v>0.5</v>
       </c>
       <c r="C7">
-        <v>2.5728600000000001E-2</v>
+        <v>9.4639000000000008E-3</v>
       </c>
       <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7">
+        <v>7.3860710000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
         <v>103</v>
       </c>
-      <c r="F7">
-        <v>-1.085777</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>104</v>
       </c>
-      <c r="E8" t="s">
-        <v>105</v>
-      </c>
       <c r="F8">
-        <v>23.465900000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+        <v>82.432980000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="39">
         <v>0.75</v>
       </c>
       <c r="C9">
-        <v>0.51879140000000001</v>
+        <v>0.48917830000000001</v>
       </c>
       <c r="D9">
-        <v>2.9860180000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+        <v>2.078751</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="39">
         <v>0.9</v>
       </c>
       <c r="C10">
-        <v>1.2561910000000001</v>
+        <v>0.91621580000000002</v>
       </c>
       <c r="D10">
-        <v>4.9187279999999998</v>
+        <v>2.9515609999999999</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F10">
-        <v>550.64859999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+        <v>6795.1970000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="39">
         <v>0.95</v>
       </c>
       <c r="C11">
-        <v>2.4095110000000002</v>
+        <v>1.69503</v>
       </c>
       <c r="D11">
-        <v>5.2888260000000002</v>
+        <v>2.9968720000000002</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F11">
-        <v>-3.647764</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+        <v>9.3188329999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="39">
         <v>0.99</v>
       </c>
       <c r="C12">
-        <v>120.896</v>
+        <v>789.47889999999995</v>
       </c>
       <c r="D12">
-        <v>120.896</v>
+        <v>789.47889999999995</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F12">
-        <v>47.83531</v>
+        <v>89.044470000000004</v>
       </c>
     </row>
   </sheetData>
@@ -2833,13 +2738,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
       <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2941,12 +2846,12 @@
       <c r="E7" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
@@ -3254,42 +3159,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="50" t="s">
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="51" t="s">
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -3301,25 +3206,25 @@
         <v>76</v>
       </c>
       <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" t="s">
         <v>117</v>
-      </c>
-      <c r="H2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" t="s">
-        <v>120</v>
       </c>
       <c r="K2" t="s">
         <v>81</v>
       </c>
       <c r="L2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N2" t="s">
         <v>66</v>
@@ -3328,19 +3233,19 @@
         <v>67</v>
       </c>
       <c r="P2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="R2" t="s">
         <v>70</v>
       </c>
       <c r="S2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="T2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U2" t="s">
         <v>73</v>
@@ -3351,7 +3256,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3359,7 +3264,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B4">
         <v>0.52429999999999999</v>
@@ -3421,7 +3326,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B8">
         <v>2.4E-2</v>
@@ -3444,7 +3349,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B9">
         <v>-1.04E-2</v>
@@ -3470,7 +3375,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B10">
         <v>5.8999999999999999E-3</v>
@@ -3499,7 +3404,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B11">
         <v>8.9999999999999998E-4</v>
@@ -3566,7 +3471,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B13">
         <v>1.2699999999999999E-2</v>
@@ -3604,7 +3509,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="42" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B14">
         <v>-0.1754</v>
@@ -3736,7 +3641,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="42" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B17">
         <v>-6.2399999999999997E-2</v>
@@ -3786,7 +3691,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B18">
         <v>-0.10829999999999999</v>
@@ -3895,7 +3800,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B20">
         <v>-1.83E-2</v>
@@ -3954,7 +3859,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="43" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B21">
         <v>-0.16220000000000001</v>
@@ -4189,12 +4094,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -4413,36 +4318,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
       <c r="AC1" s="35"/>
     </row>
     <row r="2" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4451,7 +4356,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>64</v>
@@ -4561,7 +4466,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B4" s="31">
         <v>0.51829999999999998</v>
@@ -4868,7 +4773,7 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -4897,13 +4802,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5115,13 +5020,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>